<commit_message>
add the Checkout step one robot
</commit_message>
<xml_diff>
--- a/Resources/LoginDataSauce.xlsx
+++ b/Resources/LoginDataSauce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\SauceDemo-Project\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9B7542-4772-4CB3-94EF-1AB569062C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9C764A-1FA3-4001-999E-CBAFF285077F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{97C0A37B-10FB-42B9-A061-F6A8020BCA89}"/>
   </bookViews>
@@ -429,13 +429,15 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D1" sqref="D1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>